<commit_message>
preparation publication ballot 73b1f4321e9e93e09c0c62021f543fca4c7e8bd7
</commit_message>
<xml_diff>
--- a/sd-prep-0-4-0-ballot1/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/sd-prep-0-4-0-ballot1/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -45,7 +45,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>active</t>
+    <t>draft</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-13T16:48:59+00:00</t>
+    <t>2024-05-15T13:41:06+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>